<commit_message>
added broken continue button
</commit_message>
<xml_diff>
--- a/Portfolio/Tables.xlsx
+++ b/Portfolio/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Python Code\Flash Cards Project\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3381DDE6-BBDB-450F-8937-9C7DF03AD593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B61CB-1CC5-4532-B984-4EFE52C57C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{21CC89E9-ABEF-4EE6-B08C-797DA991129C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{21CC89E9-ABEF-4EE6-B08C-797DA991129C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>IPSO</t>
   </si>
@@ -248,6 +248,35 @@
   </si>
   <si>
     <t>Test7.png</t>
+  </si>
+  <si>
+    <t>Buttons showing 
+corect answer</t>
+  </si>
+  <si>
+    <t>Test8.png</t>
+  </si>
+  <si>
+    <t>The continue buttton shoiuldn't do 
+anything untill an answer is chosen. Then it will allow the user to go to the next question.</t>
+  </si>
+  <si>
+    <t>The 3 buttons should go red/ green
+ depending on which is correct</t>
+  </si>
+  <si>
+    <t>The 3 buttons go red/ green
+ depending on which is correct</t>
+  </si>
+  <si>
+    <t>Continue button working</t>
+  </si>
+  <si>
+    <t>Test9.mp4</t>
+  </si>
+  <si>
+    <t>The continue buttton doesn't
+anything.</t>
   </si>
 </sst>
 </file>
@@ -764,16 +793,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34F6EC-96E1-408B-9A98-292AA9A3C6DD}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -924,6 +953,40 @@
       </c>
       <c r="F8" s="3" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1032,6 +1095,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0ee39083-84cb-4edb-a9c1-df561775539e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D09D92518218B7428F68173D64166B16" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7fd56902520410809d53ba577412eace">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ee39083-84cb-4edb-a9c1-df561775539e" xmlns:ns4="b25daaaa-b37a-4736-9ff5-18bede313c6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6e81dc15cfd2fd1711b120dd48b28802" ns3:_="" ns4:_="">
     <xsd:import namespace="0ee39083-84cb-4edb-a9c1-df561775539e"/>
@@ -1272,14 +1343,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0ee39083-84cb-4edb-a9c1-df561775539e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCEBCFFB-91CB-4F46-92E0-949AF4685C88}">
   <ds:schemaRefs>
@@ -1289,6 +1352,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A14DAC-1B72-4D71-83A1-A026BAEE032F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0ee39083-84cb-4edb-a9c1-df561775539e"/>
+    <ds:schemaRef ds:uri="b25daaaa-b37a-4736-9ff5-18bede313c6a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{010BC445-C0F8-4A34-97F5-A0FCE9F09E41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1305,21 +1385,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A14DAC-1B72-4D71-83A1-A026BAEE032F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0ee39083-84cb-4edb-a9c1-df561775539e"/>
-    <ds:schemaRef ds:uri="b25daaaa-b37a-4736-9ff5-18bede313c6a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>